<commit_message>
updated with scores from end of may
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
   </bookViews>
   <sheets>
-    <sheet name="jun18" sheetId="1" r:id="rId1"/>
-    <sheet name="jul18" sheetId="2" r:id="rId2"/>
+    <sheet name="may18" sheetId="3" r:id="rId1"/>
+    <sheet name="jun18" sheetId="1" r:id="rId2"/>
+    <sheet name="jul18" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="28">
   <si>
     <t>Score</t>
   </si>
@@ -101,6 +102,9 @@
   </si>
   <si>
     <t>Hole 18</t>
+  </si>
+  <si>
+    <t>Check this</t>
   </si>
 </sst>
 </file>
@@ -942,17 +946,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43275</v>
+        <v>43246</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -970,7 +977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -981,52 +988,49 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1037,12 +1041,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1051,51 +1055,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1104,7 +1108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1115,7 +1119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1123,13 +1127,13 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1137,13 +1141,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1157,37 +1161,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1196,277 +1200,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>83</v>
+        <f>SUM(B2:B19)</f>
+        <v>80</v>
       </c>
       <c r="E20">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="E37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>81</v>
-      </c>
-      <c r="E41">
-        <v>35</v>
-      </c>
+        <f>SUM(E2:E19)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1475,15 +1237,548 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>43275</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -1503,7 +1798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1517,7 +1812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1542,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1556,7 +1851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1581,7 +1876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1595,7 +1890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1606,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1620,7 +1915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1634,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1659,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1673,7 +1968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1687,7 +1982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1698,7 +1993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1712,7 +2007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1726,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1740,7 +2035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>

</xml_diff>

<commit_message>
updating scores for the 13th may
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Hole 18</t>
-  </si>
-  <si>
-    <t>Check this</t>
   </si>
 </sst>
 </file>
@@ -946,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,9 +1210,6 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
@@ -1228,7 +1222,271 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>43233</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating with scores from sunday
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="may18" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -945,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -2028,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2303,6 +2303,258 @@
         <v>32</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates for the 6th may
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="may18" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -943,18 +943,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43246</v>
       </c>
@@ -974,7 +974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -988,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>80</v>
@@ -1221,7 +1221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43233</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -1486,6 +1486,263 @@
       <c r="E41">
         <f>SUM(E23:E40)</f>
         <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1501,9 +1758,9 @@
       <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43275</v>
       </c>
@@ -1523,7 +1780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1540,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1565,7 +1822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1590,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1604,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +1875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1629,7 +1886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1643,7 +1900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1657,7 +1914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1696,7 +1953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1710,7 +1967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1721,7 +1978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1735,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1749,7 +2006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1763,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>83</v>
       </c>
@@ -1771,12 +2028,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43254</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1790,7 +2047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1801,7 +2058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1815,7 +2072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1829,7 +2086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1840,7 +2097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1868,7 +2125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1879,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1893,7 +2150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1907,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1918,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1932,7 +2189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1946,7 +2203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1960,7 +2217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1971,7 +2228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1985,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1999,7 +2256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2013,7 +2270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>81</v>
       </c>
@@ -2030,13 +2287,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -2056,7 +2313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2070,7 +2327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2081,7 +2338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2109,7 +2366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2120,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2134,7 +2391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2173,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2187,7 +2444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2198,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2212,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2226,7 +2483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2251,7 +2508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2265,7 +2522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2279,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2293,7 +2550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -2303,12 +2560,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2322,7 +2579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2333,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2347,7 +2604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2361,7 +2618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2372,7 +2629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2400,7 +2657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2411,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2425,7 +2682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2439,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2450,7 +2707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2464,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2478,7 +2735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2492,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2503,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2517,7 +2774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2531,7 +2788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2545,7 +2802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>

</xml_diff>

<commit_message>
updating with scores for the 22nd April
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
   </bookViews>
   <sheets>
-    <sheet name="may18" sheetId="3" r:id="rId1"/>
-    <sheet name="jun18" sheetId="1" r:id="rId2"/>
-    <sheet name="jul18" sheetId="2" r:id="rId3"/>
+    <sheet name="apr18" sheetId="4" r:id="rId1"/>
+    <sheet name="may18" sheetId="3" r:id="rId2"/>
+    <sheet name="jun18" sheetId="1" r:id="rId3"/>
+    <sheet name="jul18" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -943,20 +944,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43246</v>
+        <v>43212</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -974,32 +975,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1007,38 +1008,38 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1046,27 +1047,27 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1074,38 +1075,38 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1116,12 +1117,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1130,12 +1131,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1144,32 +1145,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1180,24 +1181,24 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1205,545 +1206,27 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43233</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f>SUM(B23:B40)</f>
-        <v>84</v>
-      </c>
-      <c r="E41">
-        <f>SUM(E23:E40)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>43226</v>
-      </c>
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58">
-        <v>3</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61">
-        <v>5</v>
-      </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1752,17 +1235,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43275</v>
+        <v>43246</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1780,7 +1266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1791,52 +1277,49 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1847,12 +1330,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1861,51 +1344,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1914,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1925,7 +1408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1933,13 +1416,13 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1947,13 +1430,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1967,37 +1450,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2006,64 +1489,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>83</v>
+        <f>SUM(B2:B19)</f>
+        <v>80</v>
       </c>
       <c r="E20">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SUM(E2:E19)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>43254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43233</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -2072,7 +1572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2086,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2097,60 +1597,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2164,7 +1664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2172,10 +1672,10 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2189,21 +1689,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2211,24 +1711,24 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2236,46 +1736,315 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>81</v>
-      </c>
-      <c r="E41">
-        <v>35</v>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f>SUM(B44:B61)</f>
+        <v>82</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E44:E61)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2288,12 +2057,545 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>43275</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -2313,7 +2615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2327,7 +2629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +2640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2352,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2366,7 +2668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2377,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2391,7 +2693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2405,7 +2707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2416,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2430,7 +2732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2444,7 +2746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2455,7 +2757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2469,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2483,7 +2785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2497,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2508,7 +2810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2522,7 +2824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2536,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2550,7 +2852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -2560,12 +2862,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2590,7 +2892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2604,7 +2906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2618,7 +2920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2643,7 +2945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2668,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2682,7 +2984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2696,7 +2998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +3009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2721,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2735,7 +3037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2749,7 +3051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2760,7 +3062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2774,7 +3076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2788,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2802,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>

</xml_diff>

<commit_message>
scores for the 15th april
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="apr18" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -947,15 +947,15 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43212</v>
       </c>
@@ -975,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>89</v>
@@ -1222,10 +1222,259 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -1241,12 +1490,12 @@
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43246</v>
       </c>
@@ -1266,7 +1515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1280,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1291,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1319,7 +1568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1344,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1397,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1408,7 +1657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1422,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1436,7 +1685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1450,7 +1699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1461,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1475,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1489,7 +1738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1503,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>80</v>
@@ -1513,7 +1762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43233</v>
       </c>
@@ -1533,7 +1782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1586,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1597,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1625,7 +1874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1650,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1664,7 +1913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1675,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1689,7 +1938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1703,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1717,7 +1966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1728,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1756,7 +2005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1770,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -1780,7 +2029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43226</v>
       </c>
@@ -1800,7 +2049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1814,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1825,7 +2074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1839,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1853,7 +2102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -1864,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -1878,7 +2127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -1892,7 +2141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1903,7 +2152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -1917,7 +2166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1931,7 +2180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1942,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1956,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1970,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1984,7 +2233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -1995,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -2009,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2023,7 +2272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -2037,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -2060,9 +2309,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43275</v>
       </c>
@@ -2082,7 +2331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2099,7 +2348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2124,7 +2373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2138,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2149,7 +2398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2163,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2177,7 +2426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2188,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2202,7 +2451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2216,7 +2465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2227,7 +2476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2241,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2255,7 +2504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2269,7 +2518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2280,7 +2529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2294,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2322,7 +2571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>83</v>
       </c>
@@ -2330,12 +2579,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43254</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2349,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2360,7 +2609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2374,7 +2623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2388,7 +2637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2399,7 +2648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2413,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2427,7 +2676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2438,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2452,7 +2701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2466,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2477,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2491,7 +2740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2505,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2519,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2530,7 +2779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2544,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>81</v>
       </c>
@@ -2593,9 +2842,9 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -2615,7 +2864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2629,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2640,7 +2889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2654,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2668,7 +2917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2679,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2693,7 +2942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2707,7 +2956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2718,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2732,7 +2981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2746,7 +2995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2757,7 +3006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2771,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2785,7 +3034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2799,7 +3048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2810,7 +3059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2824,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2838,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2852,7 +3101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -2862,12 +3111,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2881,7 +3130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2892,7 +3141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2906,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2920,7 +3169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2931,7 +3180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2945,7 +3194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2959,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2970,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2984,7 +3233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2998,7 +3247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3009,7 +3258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3023,7 +3272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3037,7 +3286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3051,7 +3300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3062,7 +3311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3076,7 +3325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3090,7 +3339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3104,7 +3353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>

</xml_diff>

<commit_message>
data update for 25th march 2018
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
   </bookViews>
   <sheets>
-    <sheet name="apr18" sheetId="4" r:id="rId1"/>
-    <sheet name="may18" sheetId="3" r:id="rId2"/>
-    <sheet name="jun18" sheetId="1" r:id="rId3"/>
-    <sheet name="jul18" sheetId="2" r:id="rId4"/>
+    <sheet name="mar18" sheetId="5" r:id="rId1"/>
+    <sheet name="apr18" sheetId="4" r:id="rId2"/>
+    <sheet name="may18" sheetId="3" r:id="rId3"/>
+    <sheet name="jun18" sheetId="1" r:id="rId4"/>
+    <sheet name="jul18" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -947,17 +948,17 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43212</v>
+        <v>43245</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -975,32 +976,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1011,93 +1012,69 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1106,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1117,74 +1094,74 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1192,289 +1169,40 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
         <v>25</v>
       </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f>SUM(B23:B40)</f>
-        <v>84</v>
-      </c>
-      <c r="E41">
-        <f>SUM(E23:E40)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -1484,20 +1212,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43246</v>
+        <v>43212</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1515,32 +1243,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1548,38 +1276,38 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1587,27 +1315,27 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1615,38 +1343,38 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1657,12 +1385,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1671,12 +1399,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1685,32 +1413,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1721,24 +1449,24 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1746,73 +1474,58 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>43233</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="E23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1821,21 +1534,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1846,21 +1559,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1874,18 +1587,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1893,18 +1606,18 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1913,71 +1626,71 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1991,310 +1704,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
       </c>
       <c r="E41">
         <f>SUM(E23:E40)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>43226</v>
-      </c>
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58">
-        <v>3</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61">
-        <v>5</v>
-      </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62">
-        <f>SUM(B44:B61)</f>
-        <v>82</v>
-      </c>
-      <c r="E62">
-        <f>SUM(E44:E61)</f>
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2303,17 +1752,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43275</v>
+        <v>43246</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2331,7 +1783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2342,52 +1794,49 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2398,12 +1847,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -2412,51 +1861,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -2465,7 +1914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2476,7 +1925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2484,13 +1933,13 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2498,13 +1947,13 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2518,37 +1967,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2557,64 +2006,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>83</v>
+        <f>SUM(B2:B19)</f>
+        <v>80</v>
       </c>
       <c r="E20">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SUM(E2:E19)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>43254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43233</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -2623,7 +2089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2637,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2648,60 +2114,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2715,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2723,10 +2189,10 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2740,21 +2206,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2762,24 +2228,24 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2787,46 +2253,315 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>43226</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>81</v>
-      </c>
-      <c r="E41">
-        <v>35</v>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f>SUM(B44:B61)</f>
+        <v>82</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E44:E61)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2839,12 +2574,545 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>43275</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -2864,7 +3132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2878,7 +3146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2889,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2903,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2917,7 +3185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2928,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2942,7 +3210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2956,7 +3224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2967,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2981,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2995,7 +3263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3006,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3034,7 +3302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3048,7 +3316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3059,7 +3327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3073,7 +3341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3087,7 +3355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3101,7 +3369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -3111,12 +3379,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3130,7 +3398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3141,7 +3409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3155,7 +3423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3169,7 +3437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3180,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3194,7 +3462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3208,7 +3476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3219,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3233,7 +3501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3247,7 +3515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3258,7 +3526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3272,7 +3540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3286,7 +3554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3300,7 +3568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3311,7 +3579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3325,7 +3593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3339,7 +3607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3353,7 +3621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>

</xml_diff>

<commit_message>
updating with most recent score and score from march
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F8C6DFC-6B37-48E4-97B4-749462F41B27}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mar18" sheetId="5" r:id="rId1"/>
@@ -18,12 +19,12 @@
     <sheet name="jun18" sheetId="1" r:id="rId4"/>
     <sheet name="jul18" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -944,11 +945,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,7 +959,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43245</v>
+        <v>43184</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1147,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>74</v>
@@ -1199,10 +1200,250 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>74</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -1211,10 +1452,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1751,10 +1992,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
@@ -2570,7 +2811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3103,11 +3344,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3631,6 +3872,258 @@
         <v>40</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>43295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f>SUM(B44:B61)</f>
+        <v>82</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E44:E61)</f>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
scores from feb 18
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F8C6DFC-6B37-48E4-97B4-749462F41B27}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23D02928-3D3C-49A8-8BF4-5065173C3234}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="mar18" sheetId="5" r:id="rId1"/>
-    <sheet name="apr18" sheetId="4" r:id="rId2"/>
-    <sheet name="may18" sheetId="3" r:id="rId3"/>
-    <sheet name="jun18" sheetId="1" r:id="rId4"/>
-    <sheet name="jul18" sheetId="2" r:id="rId5"/>
+    <sheet name="feb18" sheetId="6" r:id="rId1"/>
+    <sheet name="mar18" sheetId="5" r:id="rId2"/>
+    <sheet name="apr18" sheetId="4" r:id="rId3"/>
+    <sheet name="may18" sheetId="3" r:id="rId4"/>
+    <sheet name="jun18" sheetId="1" r:id="rId5"/>
+    <sheet name="jul18" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -945,10 +946,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>43184</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>74</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43149</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>59</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -1451,7 +1947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -1991,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -2810,7 +3306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -3343,7 +3839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>

</xml_diff>

<commit_message>
score update from 29th july
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23D02928-3D3C-49A8-8BF4-5065173C3234}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5B47C3E-D40A-48ED-960E-62AE4746D997}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feb18" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -949,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -3841,10 +3841,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4620,6 +4620,258 @@
         <v>31</v>
       </c>
     </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>43310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <f>SUM(B65:B82)</f>
+        <v>78</v>
+      </c>
+      <c r="E83">
+        <f>SUM(E65:E82)</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates from january golf
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5B47C3E-D40A-48ED-960E-62AE4746D997}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CAA766EA-21BF-45BA-9C07-3B9BF3EA1BFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="feb18" sheetId="6" r:id="rId1"/>
-    <sheet name="mar18" sheetId="5" r:id="rId2"/>
-    <sheet name="apr18" sheetId="4" r:id="rId3"/>
-    <sheet name="may18" sheetId="3" r:id="rId4"/>
-    <sheet name="jun18" sheetId="1" r:id="rId5"/>
-    <sheet name="jul18" sheetId="2" r:id="rId6"/>
+    <sheet name="jan 18" sheetId="7" r:id="rId1"/>
+    <sheet name="feb18" sheetId="6" r:id="rId2"/>
+    <sheet name="mar18" sheetId="5" r:id="rId3"/>
+    <sheet name="apr18" sheetId="4" r:id="rId4"/>
+    <sheet name="may18" sheetId="3" r:id="rId5"/>
+    <sheet name="jun18" sheetId="1" r:id="rId6"/>
+    <sheet name="jul18" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -946,11 +947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0DB0CF-D338-498B-A297-69FCBA60A167}">
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,60 +959,46 @@
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>43184</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43128</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1019,10 +1006,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1033,47 +1020,71 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -1082,15 +1093,18 @@
         <v>11</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1098,27 +1112,24 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1126,314 +1137,61 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
-        <f>SUM(B2:B19)</f>
-        <v>74</v>
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
       </c>
       <c r="E20">
-        <f>SUM(E2:E19)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>43149</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <f>SUM(B23:B40)</f>
-        <v>59</v>
-      </c>
-      <c r="E41">
-        <f>SUM(E23:E40)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>SUM(B3:B20)</f>
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E3:E20)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1441,10 +1199,262 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
+  <dimension ref="A2:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>SUM(B3:B20)</f>
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E3:E20)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -1947,7 +1957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -2487,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -3306,7 +3316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -3839,11 +3849,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating scored from 050818
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CAA766EA-21BF-45BA-9C07-3B9BF3EA1BFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D6AE657-7585-42A9-A6BB-2AF53E11352B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan 18" sheetId="7" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="may18" sheetId="3" r:id="rId5"/>
     <sheet name="jun18" sheetId="1" r:id="rId6"/>
     <sheet name="jul18" sheetId="2" r:id="rId7"/>
+    <sheet name="aug18" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -950,16 +951,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0DB0CF-D338-498B-A297-69FCBA60A167}">
   <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43128</v>
       </c>
@@ -979,7 +980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -993,7 +994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1135,17 +1136,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1156,17 +1157,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>60</v>
@@ -1190,7 +1191,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -1206,12 +1207,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43149</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1387,17 +1388,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1408,17 +1409,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>59</v>
@@ -1442,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -1458,12 +1459,12 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43184</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1547,22 +1548,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1696,7 +1697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>74</v>
@@ -1706,7 +1707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43178</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1790,22 +1791,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1819,7 +1820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>74</v>
@@ -1949,7 +1950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -1965,12 +1966,12 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43212</v>
       </c>
@@ -1990,7 +1991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2082,7 +2083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2174,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>89</v>
@@ -2237,12 +2238,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2320,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -2489,7 +2490,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -2505,12 +2506,12 @@
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43246</v>
       </c>
@@ -2530,7 +2531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2569,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2672,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2700,7 +2701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2739,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>80</v>
@@ -2777,7 +2778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43233</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2822,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2875,7 +2876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2914,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3006,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -3044,7 +3045,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43226</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -3128,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -3234,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -3248,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3301,7 +3302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -3324,9 +3325,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43275</v>
       </c>
@@ -3346,7 +3347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3388,7 +3389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3427,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3466,7 +3467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3519,7 +3520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3533,7 +3534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3558,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3572,7 +3573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3586,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>83</v>
       </c>
@@ -3594,12 +3595,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43254</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3613,7 +3614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3638,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3663,7 +3664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3677,7 +3678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3691,7 +3692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3769,7 +3770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3808,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>81</v>
       </c>
@@ -3853,13 +3854,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -3879,7 +3880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3893,7 +3894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3904,7 +3905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3943,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3971,7 +3972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3982,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4010,7 +4011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4035,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4074,7 +4075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4088,7 +4089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -4126,12 +4127,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -4156,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -4170,7 +4171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4195,7 +4196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -4234,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4248,7 +4249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -4287,7 +4288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4301,7 +4302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4315,7 +4316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -4354,7 +4355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4368,7 +4369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -4378,12 +4379,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43295</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -4397,7 +4398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -4408,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -4422,7 +4423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4447,7 +4448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -4475,7 +4476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -4486,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4514,7 +4515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -4525,7 +4526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -4539,7 +4540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -4553,7 +4554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -4592,7 +4593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -4606,7 +4607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -4620,7 +4621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -4630,12 +4631,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43310</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -4649,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -4660,7 +4661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -4674,7 +4675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -4699,7 +4700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -4713,7 +4714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4727,7 +4728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -4738,7 +4739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -4805,7 +4806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -4830,7 +4831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -4844,7 +4845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>25</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -4872,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83">
         <f>SUM(B65:B82)</f>
         <v>78</v>
@@ -4881,6 +4882,300 @@
         <f>SUM(E65:E82)</f>
         <v>30</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating scores from august 12
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D6AE657-7585-42A9-A6BB-2AF53E11352B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC050264-FD5F-41E1-9A81-00B5DBAD8B97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan 18" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -955,12 +955,12 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43128</v>
       </c>
@@ -980,7 +980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -994,7 +994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1136,17 +1136,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1157,17 +1157,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>60</v>
@@ -1191,7 +1191,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -1207,12 +1207,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43149</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1388,17 +1388,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1409,17 +1409,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>59</v>
@@ -1443,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -1459,12 +1459,12 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43184</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1548,22 +1548,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>74</v>
@@ -1707,7 +1707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43178</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1791,22 +1791,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>74</v>
@@ -1950,7 +1950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -1966,12 +1966,12 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43212</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>89</v>
@@ -2238,12 +2238,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -2490,7 +2490,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -2506,12 +2506,12 @@
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43246</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>80</v>
@@ -2778,7 +2778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43233</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -3045,7 +3045,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43226</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -3325,9 +3325,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43275</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>83</v>
       </c>
@@ -3595,12 +3595,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43254</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>81</v>
       </c>
@@ -3858,9 +3858,9 @@
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -4127,12 +4127,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -4379,12 +4379,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43295</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -4631,12 +4631,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>43310</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>25</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B83">
         <f>SUM(B65:B82)</f>
         <v>78</v>
@@ -4892,16 +4892,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>43317</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>83</v>
@@ -5168,13 +5168,277 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43324</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating history from dec 17
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8DBBB96-D4EB-435A-9E74-8F8706D0F42D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CBA2AC9A-C284-4D2B-8DFF-783E5BF6EB3A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="jan 18" sheetId="7" r:id="rId1"/>
-    <sheet name="feb18" sheetId="6" r:id="rId2"/>
-    <sheet name="mar18" sheetId="5" r:id="rId3"/>
-    <sheet name="apr18" sheetId="4" r:id="rId4"/>
-    <sheet name="may18" sheetId="3" r:id="rId5"/>
-    <sheet name="jun18" sheetId="1" r:id="rId6"/>
-    <sheet name="jul18" sheetId="2" r:id="rId7"/>
-    <sheet name="aug18" sheetId="8" r:id="rId8"/>
+    <sheet name="dec 17" sheetId="9" r:id="rId1"/>
+    <sheet name="jan 18" sheetId="7" r:id="rId2"/>
+    <sheet name="feb18" sheetId="6" r:id="rId3"/>
+    <sheet name="mar18" sheetId="5" r:id="rId4"/>
+    <sheet name="apr18" sheetId="4" r:id="rId5"/>
+    <sheet name="may18" sheetId="3" r:id="rId6"/>
+    <sheet name="jun18" sheetId="1" r:id="rId7"/>
+    <sheet name="jul18" sheetId="2" r:id="rId8"/>
+    <sheet name="aug18" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -948,11 +949,266 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1514A1-9ED9-4314-BB79-537C296293E3}">
+  <dimension ref="A2:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43099</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>SUM(B3:B20)</f>
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E3:E20)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0DB0CF-D338-498B-A297-69FCBA60A167}">
   <dimension ref="A2:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,7 +1686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
   <dimension ref="A2:F23"/>
   <sheetViews>
@@ -1682,7 +1938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -2189,7 +2445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -2729,7 +2985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -3548,7 +3804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -4081,7 +4337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F83"/>
   <sheetViews>
@@ -5119,7 +5375,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
   <dimension ref="A1:F64"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating scores from the past couple of weeks
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CBA2AC9A-C284-4D2B-8DFF-783E5BF6EB3A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ECC09C66-EFA9-40FD-ADAD-A135C36E489E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dec 17" sheetId="9" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="jun18" sheetId="1" r:id="rId7"/>
     <sheet name="jul18" sheetId="2" r:id="rId8"/>
     <sheet name="aug18" sheetId="8" r:id="rId9"/>
+    <sheet name="sep18" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -952,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1514A1-9ED9-4314-BB79-537C296293E3}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,6 +1198,679 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C342BDA-2ED4-46AB-AC81-0DFB76E8FC63}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>43352</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43359</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>83</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <f>SUM(B44:B61)</f>
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E44:E61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5379,8 +6053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updating scores from 14oct18
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ECC09C66-EFA9-40FD-ADAD-A135C36E489E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C13B4F31-97FD-4422-8694-DE9FFC117DA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14016" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dec 17" sheetId="9" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="jul18" sheetId="2" r:id="rId8"/>
     <sheet name="aug18" sheetId="8" r:id="rId9"/>
     <sheet name="sep18" sheetId="10" r:id="rId10"/>
+    <sheet name="oct18" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -953,16 +954,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1514A1-9ED9-4314-BB79-537C296293E3}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43099</v>
       </c>
@@ -982,7 +983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -996,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1138,17 +1139,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1159,17 +1160,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>61</v>
@@ -1193,10 +1194,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1208,16 +1209,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C342BDA-2ED4-46AB-AC81-0DFB76E8FC63}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43352</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>83</v>
@@ -1484,7 +1485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43359</v>
       </c>
@@ -1504,7 +1505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>83</v>
@@ -1751,125 +1752,419 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" t="s">
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DD3B85-208B-4E8E-B594-D6993EADE7E6}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>43387</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B62">
-        <f>SUM(B44:B61)</f>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>81</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
         <v>0</v>
       </c>
-      <c r="E62">
-        <f>SUM(E44:E61)</f>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
   </sheetData>
@@ -1885,12 +2180,12 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43128</v>
       </c>
@@ -1910,7 +2205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1924,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1935,7 +2230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1949,7 +2244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1963,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +2269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1988,7 +2283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2002,7 +2297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2027,7 +2322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2041,7 +2336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2052,7 +2347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2066,17 +2361,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2087,17 +2382,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2111,7 +2406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>60</v>
@@ -2121,10 +2416,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43114</v>
       </c>
@@ -2141,27 +2436,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2172,7 +2467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2186,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2200,7 +2495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2211,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2225,7 +2520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2239,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -2250,7 +2545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -2264,7 +2559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -2278,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2292,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -2317,7 +2612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2331,7 +2626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -2345,7 +2640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <f>SUM(B25:B42)</f>
         <v>65</v>
@@ -2368,12 +2663,12 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43149</v>
       </c>
@@ -2393,7 +2688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2407,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2418,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2432,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2446,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2457,7 +2752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2471,7 +2766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2485,7 +2780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2496,7 +2791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2510,7 +2805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2524,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2535,7 +2830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2549,17 +2844,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2570,17 +2865,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2594,7 +2889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
         <v>59</v>
@@ -2604,7 +2899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -2620,12 +2915,12 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43184</v>
       </c>
@@ -2645,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2659,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2670,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2684,7 +2979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2698,7 +2993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2709,22 +3004,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2738,7 +3033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2752,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +3058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2777,7 +3072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2791,7 +3086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2805,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2816,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2830,7 +3125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2844,7 +3139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2858,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>74</v>
@@ -2868,7 +3163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43178</v>
       </c>
@@ -2888,7 +3183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2902,7 +3197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2913,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2927,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2941,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2952,22 +3247,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2981,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2995,7 +3290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3006,7 +3301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3034,7 +3329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3048,7 +3343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3059,7 +3354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3073,7 +3368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3087,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3101,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>74</v>
@@ -3111,7 +3406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -3127,12 +3422,12 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43212</v>
       </c>
@@ -3152,7 +3447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3166,7 +3461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3177,7 +3472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3191,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3205,7 +3500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3216,7 +3511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3230,7 +3525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3244,7 +3539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3255,7 +3550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3269,7 +3564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3283,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3294,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3308,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3322,7 +3617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3336,7 +3631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3347,7 +3642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3361,7 +3656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3375,7 +3670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3389,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>89</v>
@@ -3399,12 +3694,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3418,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3429,7 +3724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3443,7 +3738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3457,7 +3752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3468,7 +3763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3482,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3496,7 +3791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3507,7 +3802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3521,7 +3816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3535,7 +3830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3546,7 +3841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -3560,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -3574,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3588,7 +3883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3599,7 +3894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3613,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3627,7 +3922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3641,7 +3936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -3651,7 +3946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
   </sheetData>
@@ -3667,12 +3962,12 @@
       <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43246</v>
       </c>
@@ -3692,7 +3987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3706,7 +4001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3717,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +4026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3745,7 +4040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3756,7 +4051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3770,7 +4065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3784,7 +4079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3795,7 +4090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3809,7 +4104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3823,7 +4118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3834,7 +4129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3848,7 +4143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -3862,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -3876,7 +4171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3887,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -3901,7 +4196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -3915,7 +4210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -3929,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>80</v>
@@ -3939,7 +4234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43233</v>
       </c>
@@ -3959,7 +4254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3973,7 +4268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3984,7 +4279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3998,7 +4293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -4012,7 +4307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4023,7 +4318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -4037,7 +4332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4051,7 +4346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -4062,7 +4357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4076,7 +4371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4090,7 +4385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4101,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -4115,7 +4410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4129,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4143,7 +4438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -4154,7 +4449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4168,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -4182,7 +4477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4196,7 +4491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -4206,7 +4501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43226</v>
       </c>
@@ -4226,7 +4521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -4240,7 +4535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -4251,7 +4546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -4265,7 +4560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4279,7 +4574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4290,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -4304,7 +4599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -4318,7 +4613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -4329,7 +4624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -4343,7 +4638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -4357,7 +4652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -4368,7 +4663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -4382,7 +4677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -4396,7 +4691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -4410,7 +4705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -4421,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -4435,7 +4730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -4449,7 +4744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -4463,7 +4758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -4486,9 +4781,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43275</v>
       </c>
@@ -4508,7 +4803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4525,7 +4820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4536,7 +4831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4550,7 +4845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4564,7 +4859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4575,7 +4870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4589,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4603,7 +4898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4614,7 +4909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4628,7 +4923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4642,7 +4937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -4653,7 +4948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4667,7 +4962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4681,7 +4976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4695,7 +4990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4706,7 +5001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4720,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4734,7 +5029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4748,7 +5043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>83</v>
       </c>
@@ -4756,12 +5051,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43254</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4775,7 +5070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -4786,7 +5081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -4800,7 +5095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -4814,7 +5109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4825,7 +5120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -4839,7 +5134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4853,7 +5148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -4864,7 +5159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4878,7 +5173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4892,7 +5187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4903,7 +5198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -4917,7 +5212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4931,7 +5226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4945,7 +5240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -4956,7 +5251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4970,7 +5265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -4984,7 +5279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4998,7 +5293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>81</v>
       </c>
@@ -5019,9 +5314,9 @@
       <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43282</v>
       </c>
@@ -5041,7 +5336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5055,7 +5350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5066,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5080,7 +5375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5094,7 +5389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -5105,7 +5400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -5119,7 +5414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5133,7 +5428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -5144,7 +5439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5158,7 +5453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -5172,7 +5467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -5183,7 +5478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -5197,7 +5492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5211,7 +5506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -5225,7 +5520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -5236,7 +5531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -5250,7 +5545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5264,7 +5559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -5278,7 +5573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>82</v>
@@ -5288,12 +5583,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43288</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -5307,7 +5602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -5318,7 +5613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -5332,7 +5627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -5346,7 +5641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -5357,7 +5652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -5371,7 +5666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -5385,7 +5680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -5396,7 +5691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -5410,7 +5705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -5424,7 +5719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5435,7 +5730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -5449,7 +5744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -5463,7 +5758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -5477,7 +5772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -5488,7 +5783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -5502,7 +5797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -5516,7 +5811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -5530,7 +5825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>84</v>
@@ -5540,12 +5835,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43295</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -5559,7 +5854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -5570,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -5584,7 +5879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -5598,7 +5893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -5609,7 +5904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -5623,7 +5918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -5637,7 +5932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -5648,7 +5943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -5662,7 +5957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -5676,7 +5971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -5687,7 +5982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -5701,7 +5996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -5715,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -5729,7 +6024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -5740,7 +6035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -5754,7 +6049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -5768,7 +6063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -5782,7 +6077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>82</v>
@@ -5792,12 +6087,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43310</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -5811,7 +6106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -5822,7 +6117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -5836,7 +6131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -5850,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -5861,7 +6156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -5875,7 +6170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -5889,7 +6184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -5900,7 +6195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -5914,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -5928,7 +6223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -5939,7 +6234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -5953,7 +6248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -5967,7 +6262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -5981,7 +6276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -5992,7 +6287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -6006,7 +6301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>25</v>
       </c>
@@ -6020,7 +6315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -6034,7 +6329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83">
         <f>SUM(B65:B82)</f>
         <v>78</v>
@@ -6057,12 +6352,12 @@
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43317</v>
       </c>
@@ -6082,7 +6377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6096,7 +6391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -6107,7 +6402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -6121,7 +6416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -6135,7 +6430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -6146,7 +6441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -6160,7 +6455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -6174,7 +6469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -6185,7 +6480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6199,7 +6494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -6213,7 +6508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -6224,7 +6519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -6238,7 +6533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -6252,7 +6547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -6266,7 +6561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -6277,7 +6572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -6291,7 +6586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -6305,7 +6600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -6319,7 +6614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>83</v>
@@ -6329,7 +6624,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43324</v>
       </c>
@@ -6349,7 +6644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -6363,7 +6658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -6374,7 +6669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -6388,7 +6683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -6402,7 +6697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -6413,7 +6708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -6427,7 +6722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -6441,7 +6736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -6452,7 +6747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -6466,7 +6761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -6480,7 +6775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -6491,7 +6786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -6505,7 +6800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -6519,7 +6814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -6533,7 +6828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -6544,7 +6839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -6558,7 +6853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -6572,7 +6867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -6586,7 +6881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f>SUM(B23:B40)</f>
         <v>81</v>
@@ -6596,7 +6891,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43331</v>
       </c>
@@ -6616,7 +6911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -6630,7 +6925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -6641,7 +6936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -6655,7 +6950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -6669,7 +6964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -6680,7 +6975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -6694,7 +6989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -6708,7 +7003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -6719,7 +7014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -6733,7 +7028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -6747,7 +7042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -6758,7 +7053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -6772,7 +7067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -6786,7 +7081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -6800,7 +7095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -6811,7 +7106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -6825,7 +7120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -6839,7 +7134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -6853,7 +7148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>SUM(B44:B61)</f>
         <v>85</v>
@@ -6863,7 +7158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating score history from the 16th November
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,29 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C13B4F31-97FD-4422-8694-DE9FFC117DA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D03C6F9-5B24-4141-A20D-CE73D8F067F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dec 17" sheetId="9" r:id="rId1"/>
-    <sheet name="jan 18" sheetId="7" r:id="rId2"/>
-    <sheet name="feb18" sheetId="6" r:id="rId3"/>
-    <sheet name="mar18" sheetId="5" r:id="rId4"/>
-    <sheet name="apr18" sheetId="4" r:id="rId5"/>
-    <sheet name="may18" sheetId="3" r:id="rId6"/>
-    <sheet name="jun18" sheetId="1" r:id="rId7"/>
-    <sheet name="jul18" sheetId="2" r:id="rId8"/>
-    <sheet name="aug18" sheetId="8" r:id="rId9"/>
-    <sheet name="sep18" sheetId="10" r:id="rId10"/>
-    <sheet name="oct18" sheetId="11" r:id="rId11"/>
+    <sheet name="nov 17" sheetId="12" r:id="rId1"/>
+    <sheet name="dec 17" sheetId="9" r:id="rId2"/>
+    <sheet name="jan 18" sheetId="7" r:id="rId3"/>
+    <sheet name="feb18" sheetId="6" r:id="rId4"/>
+    <sheet name="mar18" sheetId="5" r:id="rId5"/>
+    <sheet name="apr18" sheetId="4" r:id="rId6"/>
+    <sheet name="may18" sheetId="3" r:id="rId7"/>
+    <sheet name="jun18" sheetId="1" r:id="rId8"/>
+    <sheet name="jul18" sheetId="2" r:id="rId9"/>
+    <sheet name="aug18" sheetId="8" r:id="rId10"/>
+    <sheet name="sep18" sheetId="10" r:id="rId11"/>
+    <sheet name="oct18" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="27">
   <si>
     <t>Score</t>
   </si>
@@ -951,11 +952,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1514A1-9ED9-4314-BB79-537C296293E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6F8B1B-D102-47F6-88A2-ECD9C8B9FDD3}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +966,7 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43099</v>
+        <v>43065</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -994,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1002,7 +1003,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1019,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,10 +1028,10 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1044,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,13 +1053,13 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,10 +1070,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1108,10 +1109,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1119,10 +1120,10 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,10 +1155,10 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1175,10 +1176,10 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -1187,11 +1188,11 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>SUM(B3:B20)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E21">
         <f>SUM(E3:E20)</f>
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1206,10 +1207,832 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>83</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43324</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f>SUM(B23:B40)</f>
+        <v>81</v>
+      </c>
+      <c r="E41">
+        <f>SUM(E23:E40)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43331</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f>SUM(B44:B61)</f>
+        <v>85</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E44:E61)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C342BDA-2ED4-46AB-AC81-0DFB76E8FC63}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B62" sqref="B62:E63"/>
     </sheetView>
   </sheetViews>
@@ -1763,12 +2586,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DD3B85-208B-4E8E-B594-D6993EADE7E6}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +2814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2005,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2019,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2033,7 +2856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B2:B19)</f>
         <v>81</v>
@@ -2043,125 +2866,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f>SUM(B23:B40)</f>
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <f>SUM(E23:E40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
@@ -2173,6 +2881,261 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1514A1-9ED9-4314-BB79-537C296293E3}">
+  <dimension ref="A2:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43099</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>SUM(B3:B20)</f>
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E3:E20)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0DB0CF-D338-498B-A297-69FCBA60A167}">
   <dimension ref="A2:F43"/>
   <sheetViews>
@@ -2655,7 +3618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F64B5CB-B684-4D36-9C3B-EE8BA3DAD5A4}">
   <dimension ref="A2:F23"/>
   <sheetViews>
@@ -2907,7 +3870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -3414,7 +4377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
@@ -3954,7 +4917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -4773,7 +5736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
@@ -5306,7 +6269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F83"/>
   <sheetViews>
@@ -6342,826 +7305,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DB153A-9FAA-435F-91ED-70A97AF1F65B}">
-  <dimension ref="A1:F64"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>43317</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f>SUM(B2:B19)</f>
-        <v>83</v>
-      </c>
-      <c r="E20">
-        <f>SUM(E2:E19)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43324</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f>SUM(B23:B40)</f>
-        <v>81</v>
-      </c>
-      <c r="E41">
-        <f>SUM(E23:E40)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>43331</v>
-      </c>
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51">
-        <v>4</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52">
-        <v>4</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57">
-        <v>6</v>
-      </c>
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58">
-        <v>4</v>
-      </c>
-      <c r="E58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62">
-        <f>SUM(B44:B61)</f>
-        <v>85</v>
-      </c>
-      <c r="E62">
-        <f>SUM(E44:E61)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating from last round.
</commit_message>
<xml_diff>
--- a/Data/score_history.xlsx
+++ b/Data/score_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpaul\Documents\GitHub\OutofBounds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D03C6F9-5B24-4141-A20D-CE73D8F067F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DADBC333-569D-49C2-AB65-DC05A8E5D39C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nov 17" sheetId="12" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="aug18" sheetId="8" r:id="rId10"/>
     <sheet name="sep18" sheetId="10" r:id="rId11"/>
     <sheet name="oct18" sheetId="11" r:id="rId12"/>
+    <sheet name="nov18" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="28">
   <si>
     <t>Score</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>Hole 18</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -955,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6F8B1B-D102-47F6-88A2-ECD9C8B9FDD3}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -2590,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DD3B85-208B-4E8E-B594-D6993EADE7E6}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,6 +2868,282 @@
       <c r="E20">
         <f>SUM(E2:E19)</f>
         <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8A1998-95CE-4D6A-B59D-4B43573ACE64}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>43422</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>66</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E2:E19)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>